<commit_message>
i am trying ...
</commit_message>
<xml_diff>
--- a/data_bp/2023_tea_wt.xlsx
+++ b/data_bp/2023_tea_wt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Documents/r_projects/NREC_Decomp_2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Documents/r_projects/NREC_Decomp_2/data_bp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216B5254-C0C5-C642-90D4-0BDA5DCA185E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA876128-4509-904C-B794-10AE52D2FF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="760" windowWidth="28800" windowHeight="18000" xr2:uid="{6323B2E8-4C20-D04F-8676-F62966C64EA0}"/>
+    <workbookView xWindow="1080" yWindow="760" windowWidth="28800" windowHeight="18000" xr2:uid="{6323B2E8-4C20-D04F-8676-F62966C64EA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="12">
   <si>
     <t>tea_id</t>
   </si>
@@ -68,9 +68,6 @@
     <t>gpc</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>forgot to measure probably 2</t>
   </si>
   <si>
@@ -90,12 +87,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A516A593-0A2C-7142-8637-46791FA91D9E}">
   <dimension ref="A1:F401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A375" workbookViewId="0">
+      <selection activeCell="H381" sqref="H381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,7 +458,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -3462,8 +3466,8 @@
       <c r="D178">
         <v>7</v>
       </c>
-      <c r="E178">
-        <v>22</v>
+      <c r="E178" s="1">
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -3496,11 +3500,8 @@
       <c r="D180">
         <v>9</v>
       </c>
-      <c r="E180" t="s">
+      <c r="F180" t="s">
         <v>10</v>
-      </c>
-      <c r="F180" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
@@ -3516,11 +3517,8 @@
       <c r="D181">
         <v>10</v>
       </c>
-      <c r="E181" t="s">
+      <c r="F181" t="s">
         <v>10</v>
-      </c>
-      <c r="F181" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>